<commit_message>
corrected the timing table for the SAR
</commit_message>
<xml_diff>
--- a/config/sar/timing_table_1.xlsx
+++ b/config/sar/timing_table_1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Item</t>
   </si>
@@ -38,6 +38,24 @@
   </si>
   <si>
     <t>LSB</t>
+  </si>
+  <si>
+    <t>CB2</t>
+  </si>
+  <si>
+    <t>CB3</t>
+  </si>
+  <si>
+    <t>CB4</t>
+  </si>
+  <si>
+    <t>CB5</t>
+  </si>
+  <si>
+    <t>CB6</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -88,9 +106,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -398,16 +422,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="25.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -438,6 +462,52 @@
         <v>7</v>
       </c>
     </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>